<commit_message>
Colorz wieder ohne description
</commit_message>
<xml_diff>
--- a/data/colors.xlsx
+++ b/data/colors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franziska\Desktop\Info_Passwords\Sketches\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franziska\Desktop\Info_Passwords\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>animal</t>
   </si>
@@ -84,36 +84,6 @@
   </si>
   <si>
     <t>#65FF61</t>
-  </si>
-  <si>
-    <t>using personal names</t>
-  </si>
-  <si>
-    <t>fruits, fast food etc.</t>
-  </si>
-  <si>
-    <t>insulting or rude words</t>
-  </si>
-  <si>
-    <t>self-related, kind of arrogant</t>
-  </si>
-  <si>
-    <t>references to star wars etc.</t>
-  </si>
-  <si>
-    <t>cute things like cats</t>
-  </si>
-  <si>
-    <t>sport-related words</t>
-  </si>
-  <si>
-    <t>related to the term password</t>
-  </si>
-  <si>
-    <t>using letters and numbers</t>
-  </si>
-  <si>
-    <t>using animal names</t>
   </si>
 </sst>
 </file>
@@ -465,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C88A97-C669-4369-8746-923386491045}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,144 +447,84 @@
     <col min="3" max="3" width="26.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10">
-        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>